<commit_message>
Fix issues to identify selected Map-Items...  Started the implementation of the Delete functionality.
</commit_message>
<xml_diff>
--- a/Documentation/Mapping.Samples.xlsx
+++ b/Documentation/Mapping.Samples.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prjs\Datovy.Edam\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A7CFEC0-60B5-4E29-BA7E-7DE8B42C6495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD16AAC-612B-4E02-A00A-17DA2C2FB53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22245" yWindow="7680" windowWidth="24945" windowHeight="19335" xr2:uid="{589AA2A9-EAA1-4E71-B4C2-E66F08A5A0B8}"/>
+    <workbookView xWindow="9570" yWindow="2310" windowWidth="34155" windowHeight="18690" xr2:uid="{589AA2A9-EAA1-4E71-B4C2-E66F08A5A0B8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapping Samples" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -181,11 +181,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,7 +491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -503,7 +502,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,15 +595,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>

</xml_diff>